<commit_message>
added the 15 new repos
</commit_message>
<xml_diff>
--- a/data/labeled_dataset_repos.xlsx
+++ b/data/labeled_dataset_repos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\const\Documents\Bachelorarbeit\bachelor_repo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\const\Documents\Bachelorarbeit\bachelor_repo\github-classifier\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA614854-9C69-4EEF-BBF1-49931754C339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78035A6-DE22-4F88-ABE0-8482138A67E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="720" windowWidth="21750" windowHeight="15480" xr2:uid="{22739A3E-992F-4298-AA9B-BA6D95F139BF}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21750" windowHeight="15480" xr2:uid="{22739A3E-992F-4298-AA9B-BA6D95F139BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="377">
   <si>
     <t>html_url</t>
   </si>
@@ -1044,6 +1044,129 @@
   </si>
   <si>
     <t>A clean and simple data loading library for Continual Learning</t>
+  </si>
+  <si>
+    <t>https://github.com/MASILab/3DUX-Net</t>
+  </si>
+  <si>
+    <t>https://github.com/yifita/DSS</t>
+  </si>
+  <si>
+    <t>differentiable-renderer|differentiable-rendering|geometry-processing|inverse-rendering|point-cloud|rendering|siggraph-asia</t>
+  </si>
+  <si>
+    <t>Differentiable Surface Splatting</t>
+  </si>
+  <si>
+    <t>https://github.com/brentyi/tyro</t>
+  </si>
+  <si>
+    <t>argparse|argument-parsing|dataclasses</t>
+  </si>
+  <si>
+    <t>Strongly typed, zero-effort CLI interfaces &amp; config objects</t>
+  </si>
+  <si>
+    <t>https://github.com/AutoViML/Auto_ViML</t>
+  </si>
+  <si>
+    <t>auto-viml|autokeras|automated-machine-learning|automl|automl-algorithms|autosklearn|machine-learning|python|python3|scikit-learn|tpot|xgboost</t>
+  </si>
+  <si>
+    <t>Automatically Build Multiple ML Models with a Single Line of Code. Created by Ram Seshadri. Collaborators Welcome. Permission Granted upon Request.</t>
+  </si>
+  <si>
+    <t>https://github.com/DataCanvasIO/Hypernets</t>
+  </si>
+  <si>
+    <t>autodl|automl|enas|evolutionary-algorithms|hyperparameter-optimization|hyperparameter-tuning|keras|mcts|monte-carlo-tree-search|nas|nasnet|neural-architecture-search|reinforcement-learning</t>
+  </si>
+  <si>
+    <t>A General Automated Machine Learning framework to simplify the development of End-to-end AutoML toolkits in specific domains.</t>
+  </si>
+  <si>
+    <t>https://github.com/showlab/Vlog</t>
+  </si>
+  <si>
+    <t>chatgpt|langchain|large-language-model|video-language|whisper</t>
+  </si>
+  <si>
+    <t>Transform Video as a Document with ChatGPT, CLIP, BLIP2, GRIT, Whisper, LangChain.</t>
+  </si>
+  <si>
+    <t>https://github.com/tensorflow/datasets</t>
+  </si>
+  <si>
+    <t>data|dataset|datasets|jax|machine-learning|numpy|tensorflow</t>
+  </si>
+  <si>
+    <t>TFDS is a collection of datasets ready to use with TensorFlow, Jax, ...</t>
+  </si>
+  <si>
+    <t>https://github.com/cwlroda/falldetection_openpifpaf</t>
+  </si>
+  <si>
+    <t>composite-fields|computer-vision|cpu|deep-learning|detection|fall-detection|gpu|human-pose-estimation|object-tracking|openpifpaf|video-analytics</t>
+  </si>
+  <si>
+    <t>Fall Detection using OpenPifPaf's Human Pose Estimation model</t>
+  </si>
+  <si>
+    <t>https://github.com/7eu7d7/DreamArtist-stable-diffusion</t>
+  </si>
+  <si>
+    <t>stable diffusion webui with contrastive prompt tuning</t>
+  </si>
+  <si>
+    <t>https://github.com/Bismuth-Consultancy-BV/MLOPs</t>
+  </si>
+  <si>
+    <t>Machine Learning Toolset for Houdini</t>
+  </si>
+  <si>
+    <t>https://github.com/YingqingHe/LVDM</t>
+  </si>
+  <si>
+    <t>LVDM: Latent Video Diffusion Models for High-Fidelity Long Video Generation</t>
+  </si>
+  <si>
+    <t>https://github.com/YuliangXiu/ICON</t>
+  </si>
+  <si>
+    <t>3d-reconstruction|animation|avatar-generator|cloth-simulation|computer-graphics|computer-vision|human-pose-estimation|implicit-functions|mesh-deformation|metaverse|normal-maps|pifu|pifuhd|pose-estimation|pytorch|smpl|smpl-body|smpl-model|smplx|virtual-humans</t>
+  </si>
+  <si>
+    <t>[CVPR'22] ICON: Implicit Clothed humans Obtained from Normals</t>
+  </si>
+  <si>
+    <t>https://github.com/webis-de/small-text</t>
+  </si>
+  <si>
+    <t>active-learning|deep-learning|looking-for-contributors|machine-learning|natural-language-processing|nlp|python|pytorch|text-classification|transformers</t>
+  </si>
+  <si>
+    <t>Active Learning for Text Classification in Python</t>
+  </si>
+  <si>
+    <t>https://github.com/modelscope/modelscope</t>
+  </si>
+  <si>
+    <t>cv|deep-learning|machine-learning|multi-modal|nlp|python|science|speech</t>
+  </si>
+  <si>
+    <t>ModelScope: bring the notion of Model-as-a-Service to life.</t>
+  </si>
+  <si>
+    <t>https://github.com/huggingface/optimum-intel</t>
+  </si>
+  <si>
+    <t>diffusers|distillation|inference|intel|onnx|openvino|optimization|pruning|quantization|transformers</t>
+  </si>
+  <si>
+    <t>������������ Optimum Intel: Accelerate inference with Intel optimization tools</t>
+  </si>
+  <si>
+    <t>Plugin</t>
   </si>
 </sst>
 </file>
@@ -1096,12 +1219,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1437,16 +1560,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65A8AEA-A0A5-4449-B988-53D5AD057A76}">
-  <dimension ref="A1:AMJ116"/>
+  <dimension ref="A1:AMJ131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
     <col min="11" max="11" width="26.85546875" customWidth="1"/>
     <col min="12" max="12" width="19.140625" customWidth="1"/>
     <col min="13" max="13" width="18.7109375" customWidth="1"/>
@@ -1492,17 +1615,17 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1593,15 +1716,15 @@
       </c>
       <c r="N3">
         <f>COUNTIF(J:J, "*"&amp;N2&amp;"*")</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <f>COUNTIF(J:J, "*"&amp;O2&amp;"*")</f>
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="P3">
         <f>COUNTIF(J:J, "*"&amp;P2&amp;"*")</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="Q3">
         <f>COUNTIF(J:J, "*"&amp;Q2&amp;"*")</f>
@@ -1609,15 +1732,15 @@
       </c>
       <c r="R3">
         <f>COUNTIF(K:K, "*"&amp;R2&amp;"*")</f>
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="S3">
         <f>COUNTIF(K:K, "*"&amp;S2&amp;"*")</f>
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="T3">
         <f>COUNTIF(K:K, "*"&amp;T2&amp;"*")</f>
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1654,33 +1777,33 @@
       <c r="K4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <f t="shared" ref="N4:T4" si="0">N3/100</f>
-        <v>0.22</v>
-      </c>
-      <c r="O4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="O4" s="1">
         <f t="shared" si="0"/>
-        <v>0.81</v>
-      </c>
-      <c r="P4" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="P4" s="1">
         <f t="shared" si="0"/>
-        <v>0.16</v>
-      </c>
-      <c r="Q4" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="Q4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="1">
         <f t="shared" si="0"/>
-        <v>0.46</v>
-      </c>
-      <c r="S4" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="S4" s="1">
         <f t="shared" si="0"/>
-        <v>0.52</v>
-      </c>
-      <c r="T4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="T4" s="1">
         <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -4912,38 +5035,38 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:1024" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:1024" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="2">
         <v>901</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D100" s="3" t="s">
+      <c r="C100" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E100" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F100" s="3">
+      <c r="F100" s="2">
         <v>10510</v>
       </c>
-      <c r="G100" s="3">
+      <c r="G100" s="2">
         <v>170</v>
       </c>
-      <c r="H100" s="3">
+      <c r="H100" s="2">
         <v>9</v>
       </c>
-      <c r="I100" s="3">
+      <c r="I100" s="2">
         <v>24</v>
       </c>
-      <c r="J100" s="3" t="s">
+      <c r="J100" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K100" s="3" t="s">
+      <c r="K100" s="2" t="s">
         <v>19</v>
       </c>
       <c r="ALV100"/>
@@ -4998,7 +5121,7 @@
       </c>
     </row>
     <row r="102" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="3" t="s">
         <v>298</v>
       </c>
       <c r="B102">
@@ -5039,7 +5162,7 @@
       </c>
     </row>
     <row r="103" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
+      <c r="A103" s="3" t="s">
         <v>301</v>
       </c>
       <c r="B103">
@@ -5074,7 +5197,7 @@
       </c>
     </row>
     <row r="104" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
+      <c r="A104" s="3" t="s">
         <v>302</v>
       </c>
       <c r="B104">
@@ -5112,7 +5235,7 @@
       </c>
     </row>
     <row r="105" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="3" t="s">
         <v>304</v>
       </c>
       <c r="B105">
@@ -5153,7 +5276,7 @@
       </c>
     </row>
     <row r="106" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
+      <c r="A106" s="3" t="s">
         <v>307</v>
       </c>
       <c r="B106">
@@ -5194,7 +5317,7 @@
       </c>
     </row>
     <row r="107" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="3" t="s">
         <v>310</v>
       </c>
       <c r="B107">
@@ -5232,7 +5355,7 @@
       </c>
     </row>
     <row r="108" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
+      <c r="A108" s="3" t="s">
         <v>312</v>
       </c>
       <c r="B108">
@@ -5270,7 +5393,7 @@
       </c>
     </row>
     <row r="109" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+      <c r="A109" s="3" t="s">
         <v>314</v>
       </c>
       <c r="B109">
@@ -5311,7 +5434,7 @@
       </c>
     </row>
     <row r="110" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+      <c r="A110" s="3" t="s">
         <v>317</v>
       </c>
       <c r="B110">
@@ -5349,7 +5472,7 @@
       </c>
     </row>
     <row r="111" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="3" t="s">
         <v>319</v>
       </c>
       <c r="B111">
@@ -5390,7 +5513,7 @@
       </c>
     </row>
     <row r="112" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="3" t="s">
         <v>322</v>
       </c>
       <c r="B112">
@@ -5428,7 +5551,7 @@
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
+      <c r="A113" s="3" t="s">
         <v>324</v>
       </c>
       <c r="B113">
@@ -5469,7 +5592,7 @@
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
+      <c r="A114" s="3" t="s">
         <v>327</v>
       </c>
       <c r="B114">
@@ -5510,7 +5633,7 @@
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
+      <c r="A115" s="3" t="s">
         <v>330</v>
       </c>
       <c r="B115">
@@ -5551,7 +5674,7 @@
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
+      <c r="A116" s="3" t="s">
         <v>333</v>
       </c>
       <c r="B116">
@@ -5589,6 +5712,606 @@
       </c>
       <c r="M116" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B117">
+        <v>162</v>
+      </c>
+      <c r="C117" t="s">
+        <v>16</v>
+      </c>
+      <c r="F117">
+        <v>27366</v>
+      </c>
+      <c r="G117">
+        <v>252</v>
+      </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117">
+        <v>10</v>
+      </c>
+      <c r="J117" t="s">
+        <v>18</v>
+      </c>
+      <c r="K117" t="s">
+        <v>19</v>
+      </c>
+      <c r="L117" t="s">
+        <v>21</v>
+      </c>
+      <c r="M117" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B118">
+        <v>330</v>
+      </c>
+      <c r="C118" t="s">
+        <v>16</v>
+      </c>
+      <c r="D118" t="s">
+        <v>338</v>
+      </c>
+      <c r="E118" t="s">
+        <v>339</v>
+      </c>
+      <c r="F118">
+        <v>7347</v>
+      </c>
+      <c r="G118">
+        <v>59</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <v>5</v>
+      </c>
+      <c r="J118" t="s">
+        <v>18</v>
+      </c>
+      <c r="K118" t="s">
+        <v>23</v>
+      </c>
+      <c r="L118" t="s">
+        <v>21</v>
+      </c>
+      <c r="M118" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B119">
+        <v>257</v>
+      </c>
+      <c r="C119" t="s">
+        <v>16</v>
+      </c>
+      <c r="D119" t="s">
+        <v>341</v>
+      </c>
+      <c r="E119" t="s">
+        <v>342</v>
+      </c>
+      <c r="F119">
+        <v>14726</v>
+      </c>
+      <c r="G119">
+        <v>115</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119">
+        <v>1</v>
+      </c>
+      <c r="J119" t="s">
+        <v>21</v>
+      </c>
+      <c r="K119" t="s">
+        <v>24</v>
+      </c>
+      <c r="L119" t="s">
+        <v>18</v>
+      </c>
+      <c r="M119" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B120">
+        <v>471</v>
+      </c>
+      <c r="C120" t="s">
+        <v>16</v>
+      </c>
+      <c r="D120" t="s">
+        <v>344</v>
+      </c>
+      <c r="E120" t="s">
+        <v>345</v>
+      </c>
+      <c r="F120">
+        <v>7402</v>
+      </c>
+      <c r="G120">
+        <v>14</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>4</v>
+      </c>
+      <c r="J120" t="s">
+        <v>21</v>
+      </c>
+      <c r="K120" t="s">
+        <v>280</v>
+      </c>
+      <c r="L120" t="s">
+        <v>21</v>
+      </c>
+      <c r="M120" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B121">
+        <v>245</v>
+      </c>
+      <c r="C121" t="s">
+        <v>16</v>
+      </c>
+      <c r="D121" t="s">
+        <v>347</v>
+      </c>
+      <c r="E121" t="s">
+        <v>348</v>
+      </c>
+      <c r="F121">
+        <v>28311</v>
+      </c>
+      <c r="G121">
+        <v>274</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>48</v>
+      </c>
+      <c r="J121" t="s">
+        <v>21</v>
+      </c>
+      <c r="K121" t="s">
+        <v>24</v>
+      </c>
+      <c r="L121" t="s">
+        <v>18</v>
+      </c>
+      <c r="M121" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B122">
+        <v>422</v>
+      </c>
+      <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" t="s">
+        <v>350</v>
+      </c>
+      <c r="E122" t="s">
+        <v>351</v>
+      </c>
+      <c r="F122">
+        <v>34594</v>
+      </c>
+      <c r="G122">
+        <v>329</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>12</v>
+      </c>
+      <c r="J122" t="s">
+        <v>20</v>
+      </c>
+      <c r="K122" t="s">
+        <v>19</v>
+      </c>
+      <c r="L122" t="s">
+        <v>20</v>
+      </c>
+      <c r="M122" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B123">
+        <v>4032</v>
+      </c>
+      <c r="C123" t="s">
+        <v>16</v>
+      </c>
+      <c r="D123" t="s">
+        <v>353</v>
+      </c>
+      <c r="E123" t="s">
+        <v>354</v>
+      </c>
+      <c r="F123">
+        <v>96311</v>
+      </c>
+      <c r="G123">
+        <v>1587</v>
+      </c>
+      <c r="H123">
+        <v>19</v>
+      </c>
+      <c r="I123">
+        <v>14949</v>
+      </c>
+      <c r="J123" t="s">
+        <v>18</v>
+      </c>
+      <c r="K123" t="s">
+        <v>24</v>
+      </c>
+      <c r="L123" t="s">
+        <v>18</v>
+      </c>
+      <c r="M123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B124">
+        <v>286</v>
+      </c>
+      <c r="C124" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" t="s">
+        <v>356</v>
+      </c>
+      <c r="E124" t="s">
+        <v>357</v>
+      </c>
+      <c r="F124">
+        <v>22882</v>
+      </c>
+      <c r="G124">
+        <v>92</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>66</v>
+      </c>
+      <c r="J124" t="s">
+        <v>148</v>
+      </c>
+      <c r="K124" t="s">
+        <v>19</v>
+      </c>
+      <c r="L124" t="s">
+        <v>20</v>
+      </c>
+      <c r="M124" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B125">
+        <v>861</v>
+      </c>
+      <c r="C125" t="s">
+        <v>16</v>
+      </c>
+      <c r="E125" t="s">
+        <v>359</v>
+      </c>
+      <c r="F125">
+        <v>12385</v>
+      </c>
+      <c r="G125">
+        <v>97</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>44</v>
+      </c>
+      <c r="J125" t="s">
+        <v>20</v>
+      </c>
+      <c r="K125" t="s">
+        <v>19</v>
+      </c>
+      <c r="L125" t="s">
+        <v>20</v>
+      </c>
+      <c r="M125" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B126">
+        <v>279</v>
+      </c>
+      <c r="C126" t="s">
+        <v>16</v>
+      </c>
+      <c r="E126" t="s">
+        <v>361</v>
+      </c>
+      <c r="F126">
+        <v>6902</v>
+      </c>
+      <c r="G126">
+        <v>78</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <v>193</v>
+      </c>
+      <c r="J126" t="s">
+        <v>376</v>
+      </c>
+      <c r="K126" t="s">
+        <v>19</v>
+      </c>
+      <c r="L126" t="s">
+        <v>18</v>
+      </c>
+      <c r="M126" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B127">
+        <v>327</v>
+      </c>
+      <c r="C127" t="s">
+        <v>16</v>
+      </c>
+      <c r="E127" t="s">
+        <v>363</v>
+      </c>
+      <c r="F127">
+        <v>6168</v>
+      </c>
+      <c r="G127">
+        <v>40</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>3</v>
+      </c>
+      <c r="J127" t="s">
+        <v>18</v>
+      </c>
+      <c r="K127" t="s">
+        <v>23</v>
+      </c>
+      <c r="L127" t="s">
+        <v>21</v>
+      </c>
+      <c r="M127" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B128">
+        <v>1471</v>
+      </c>
+      <c r="C128" t="s">
+        <v>16</v>
+      </c>
+      <c r="D128" t="s">
+        <v>365</v>
+      </c>
+      <c r="E128" t="s">
+        <v>366</v>
+      </c>
+      <c r="F128">
+        <v>22540</v>
+      </c>
+      <c r="G128">
+        <v>146</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>33</v>
+      </c>
+      <c r="J128" t="s">
+        <v>18</v>
+      </c>
+      <c r="K128" t="s">
+        <v>19</v>
+      </c>
+      <c r="L128" t="s">
+        <v>21</v>
+      </c>
+      <c r="M128" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B129">
+        <v>500</v>
+      </c>
+      <c r="C129" t="s">
+        <v>16</v>
+      </c>
+      <c r="D129" t="s">
+        <v>368</v>
+      </c>
+      <c r="E129" t="s">
+        <v>369</v>
+      </c>
+      <c r="F129">
+        <v>14618</v>
+      </c>
+      <c r="G129">
+        <v>200</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <v>6</v>
+      </c>
+      <c r="J129" t="s">
+        <v>18</v>
+      </c>
+      <c r="K129" t="s">
+        <v>23</v>
+      </c>
+      <c r="L129" t="s">
+        <v>18</v>
+      </c>
+      <c r="M129" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B130">
+        <v>4474</v>
+      </c>
+      <c r="C130" t="s">
+        <v>16</v>
+      </c>
+      <c r="D130" t="s">
+        <v>371</v>
+      </c>
+      <c r="E130" t="s">
+        <v>372</v>
+      </c>
+      <c r="F130">
+        <v>375129</v>
+      </c>
+      <c r="G130">
+        <v>3131</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>35</v>
+      </c>
+      <c r="J130" t="s">
+        <v>18</v>
+      </c>
+      <c r="K130" t="s">
+        <v>19</v>
+      </c>
+      <c r="L130" t="s">
+        <v>18</v>
+      </c>
+      <c r="M130" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B131">
+        <v>221</v>
+      </c>
+      <c r="C131" t="s">
+        <v>16</v>
+      </c>
+      <c r="D131" t="s">
+        <v>374</v>
+      </c>
+      <c r="E131" t="s">
+        <v>375</v>
+      </c>
+      <c r="F131">
+        <v>22653</v>
+      </c>
+      <c r="G131">
+        <v>100</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>28</v>
+      </c>
+      <c r="J131" t="s">
+        <v>21</v>
+      </c>
+      <c r="K131" t="s">
+        <v>24</v>
+      </c>
+      <c r="L131" t="s">
+        <v>148</v>
+      </c>
+      <c r="M131" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5612,6 +6335,21 @@
     <hyperlink ref="A114" r:id="rId13" xr:uid="{111E205A-6FEA-4274-ABCE-7EA64B449554}"/>
     <hyperlink ref="A115" r:id="rId14" xr:uid="{EC136369-C93F-4579-9368-5607D1D19639}"/>
     <hyperlink ref="A116" r:id="rId15" xr:uid="{F6DAA306-2575-4095-B428-C81B15965E81}"/>
+    <hyperlink ref="A117" r:id="rId16" xr:uid="{F5B08C98-EAA1-4923-AA32-5F795E86E5AD}"/>
+    <hyperlink ref="A118" r:id="rId17" xr:uid="{A483A1C3-191F-4357-BF6A-C4BDA386CD60}"/>
+    <hyperlink ref="A119" r:id="rId18" xr:uid="{820FBDE5-4973-4EC0-8460-C4D4FA3F03AC}"/>
+    <hyperlink ref="A120" r:id="rId19" xr:uid="{CD2832FC-13F4-4B74-B7F1-9208F6FB5893}"/>
+    <hyperlink ref="A121" r:id="rId20" xr:uid="{1F040FC6-C180-46DF-BBFB-15C7CD0CE248}"/>
+    <hyperlink ref="A122" r:id="rId21" xr:uid="{73023670-C966-45A5-A88C-BDE66C22E31A}"/>
+    <hyperlink ref="A123" r:id="rId22" xr:uid="{E7909988-9FA1-41A1-A80E-87C2BA2B5056}"/>
+    <hyperlink ref="A124" r:id="rId23" xr:uid="{C60FE6ED-043E-4034-ACA0-44AC10366079}"/>
+    <hyperlink ref="A125" r:id="rId24" xr:uid="{4805E4D9-D135-4BA8-B899-9925D6204896}"/>
+    <hyperlink ref="A126" r:id="rId25" xr:uid="{21A67361-311A-4191-ACB9-D10251F332E9}"/>
+    <hyperlink ref="A127" r:id="rId26" xr:uid="{A776CE6C-EC16-4700-A62D-D846A12C1B10}"/>
+    <hyperlink ref="A128" r:id="rId27" xr:uid="{4865879A-1C3D-4067-91D2-C0F530C63F92}"/>
+    <hyperlink ref="A129" r:id="rId28" xr:uid="{DE118CB6-F21E-42A2-B872-D6BC8CE3EFAF}"/>
+    <hyperlink ref="A130" r:id="rId29" xr:uid="{E291CD9D-C495-432E-8AFB-975B0EE65555}"/>
+    <hyperlink ref="A131" r:id="rId30" xr:uid="{3DE1EB34-2770-4DCE-AB53-86E5468D07FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>